<commit_message>
Added missing HPs in the Nile from AHA and REPP
</commit_message>
<xml_diff>
--- a/HydroFPV_plants/CombinedTechsCreation/CapacityFactors_solar.xlsx
+++ b/HydroFPV_plants/CombinedTechsCreation/CapacityFactors_solar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TUDELFT\THESIS\Data\Global solar atlas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro Pieruzzi\Documents\Thesis\TEMBA_FPV\HydroFPV_plants\CombinedTechsCreation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EC81B0-3664-4E68-83D7-A6747BA19FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AEAC8D-755F-4981-9AAA-E9BB7D006695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>loc_name</t>
   </si>
@@ -62,58 +62,118 @@
     <t>s4d2</t>
   </si>
   <si>
+    <t>AleltuEast</t>
+  </si>
+  <si>
+    <t>AleltuWest</t>
+  </si>
+  <si>
+    <t>AmarthiNeshe</t>
+  </si>
+  <si>
+    <t>Aswan1</t>
+  </si>
+  <si>
+    <t>Aswan2</t>
+  </si>
+  <si>
+    <t>Baro</t>
+  </si>
+  <si>
+    <t>BekoAbo</t>
+  </si>
+  <si>
+    <t>Birbir</t>
+  </si>
+  <si>
+    <t>ChemogaYeda</t>
+  </si>
+  <si>
+    <t>Dagash</t>
+  </si>
+  <si>
+    <t>Dal</t>
+  </si>
+  <si>
+    <t>Finchaa</t>
+  </si>
+  <si>
+    <t>Geba</t>
+  </si>
+  <si>
+    <t>Genji</t>
+  </si>
+  <si>
     <t>HighAswan</t>
   </si>
   <si>
-    <t>Aswan</t>
+    <t>JebelAulia</t>
+  </si>
+  <si>
+    <t>JubaBarrage</t>
+  </si>
+  <si>
+    <t>Kajbar</t>
+  </si>
+  <si>
+    <t>Karadobi</t>
+  </si>
+  <si>
+    <t>KashElGirba</t>
+  </si>
+  <si>
+    <t>LakeTana</t>
+  </si>
+  <si>
+    <t>LowerDabus</t>
+  </si>
+  <si>
+    <t>LowerDedessa</t>
+  </si>
+  <si>
+    <t>Merowe</t>
+  </si>
+  <si>
+    <t>Mograt</t>
   </si>
   <si>
     <t>Renaissance</t>
   </si>
   <si>
+    <t>Roseires</t>
+  </si>
+  <si>
+    <t>Sabaloka</t>
+  </si>
+  <si>
+    <t>Sennar</t>
+  </si>
+  <si>
+    <t>Shereik</t>
+  </si>
+  <si>
+    <t>Sor2</t>
+  </si>
+  <si>
+    <t>Tams</t>
+  </si>
+  <si>
+    <t>Tekeze1</t>
+  </si>
+  <si>
+    <t>Tekeze2</t>
+  </si>
+  <si>
+    <t>UpperAtbara</t>
+  </si>
+  <si>
+    <t>UpperDabus</t>
+  </si>
+  <si>
     <t>UpperMandaya</t>
   </si>
   <si>
-    <t>Karadobi</t>
-  </si>
-  <si>
-    <t>BekoAbo</t>
-  </si>
-  <si>
-    <t>ChemogaYeda</t>
-  </si>
-  <si>
-    <t>Merowe</t>
-  </si>
-  <si>
-    <t>Roseires</t>
-  </si>
-  <si>
-    <t>Sennar</t>
-  </si>
-  <si>
-    <t>JebelAulia</t>
-  </si>
-  <si>
-    <t>Dal</t>
-  </si>
-  <si>
-    <t>Shereik</t>
-  </si>
-  <si>
-    <t>Kajbar</t>
-  </si>
-  <si>
-    <t>Dagash</t>
-  </si>
-  <si>
-    <t>Mograt</t>
-  </si>
-  <si>
-    <t>Sabaloka</t>
-  </si>
-  <si>
-    <t>LakeTana</t>
+    <t>Wau</t>
   </si>
 </sst>
 </file>
@@ -132,7 +192,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -477,13 +536,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y28"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -522,28 +584,28 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>0.40586848506571083</v>
+        <v>0.28975484309040223</v>
       </c>
       <c r="D2">
-        <v>0.12603861242532849</v>
+        <v>0.13667612353643971</v>
       </c>
       <c r="E2">
-        <v>0.38385520469932288</v>
+        <v>0.2641995675029869</v>
       </c>
       <c r="F2">
-        <v>0.11816489581839899</v>
+        <v>9.4938511350059748E-2</v>
       </c>
       <c r="G2">
-        <v>0.37423852608522501</v>
+        <v>0.29161254161688599</v>
       </c>
       <c r="H2">
-        <v>0.1297939178016726</v>
+        <v>0.13333808936678609</v>
       </c>
       <c r="I2">
-        <v>0.39426057176992663</v>
+        <v>0.35088009813961418</v>
       </c>
       <c r="J2">
-        <v>0.1117774126984127</v>
+        <v>0.14635089605734769</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -554,28 +616,28 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>0.40949003026682601</v>
+        <v>0.28975484309040223</v>
       </c>
       <c r="D3">
-        <v>0.1261858979689367</v>
+        <v>0.13667612353643971</v>
       </c>
       <c r="E3">
-        <v>0.38181073277578648</v>
+        <v>0.2641995675029869</v>
       </c>
       <c r="F3">
-        <v>0.1174411816009558</v>
+        <v>9.4938511350059748E-2</v>
       </c>
       <c r="G3">
-        <v>0.37100408442851451</v>
+        <v>0.29161254161688571</v>
       </c>
       <c r="H3">
-        <v>0.1288478107526882</v>
+        <v>0.13333808936678609</v>
       </c>
       <c r="I3">
-        <v>0.4012607561017239</v>
+        <v>0.35088009813961418</v>
       </c>
       <c r="J3">
-        <v>0.1126826774193548</v>
+        <v>0.14635089605734769</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -586,28 +648,28 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>0.33303783671843878</v>
+        <v>0.32822893986459573</v>
       </c>
       <c r="D4">
-        <v>0.10567916917562729</v>
+        <v>0.11213200095579449</v>
       </c>
       <c r="E4">
-        <v>0.27764846395858228</v>
+        <v>0.25394759219434487</v>
       </c>
       <c r="F4">
-        <v>6.7827279569892471E-2</v>
+        <v>7.8348711589008357E-2</v>
       </c>
       <c r="G4">
-        <v>0.30851121903624051</v>
+        <v>0.30030267144563932</v>
       </c>
       <c r="H4">
-        <v>0.1091898138590203</v>
+        <v>0.11891993715651129</v>
       </c>
       <c r="I4">
-        <v>0.37835753840245773</v>
+        <v>0.38199672683051711</v>
       </c>
       <c r="J4">
-        <v>0.11339636354326681</v>
+        <v>0.1325895962621608</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -618,28 +680,28 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>0.32756912345679012</v>
+        <v>0.40949003026682601</v>
       </c>
       <c r="D5">
-        <v>9.7332529988052571E-2</v>
+        <v>0.1261858979689367</v>
       </c>
       <c r="E5">
-        <v>0.26230201513341289</v>
+        <v>0.38181073277578648</v>
       </c>
       <c r="F5">
-        <v>7.0104277419354835E-2</v>
+        <v>0.1174411816009558</v>
       </c>
       <c r="G5">
-        <v>0.32110683074472318</v>
+        <v>0.37100408442851451</v>
       </c>
       <c r="H5">
-        <v>0.10273956296296299</v>
+        <v>0.1288478107526882</v>
       </c>
       <c r="I5">
-        <v>0.37596370327700979</v>
+        <v>0.4012607561017239</v>
       </c>
       <c r="J5">
-        <v>0.111860513312852</v>
+        <v>0.1126826774193548</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -650,28 +712,28 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>0.34185133452807648</v>
+        <v>0.40949003026682601</v>
       </c>
       <c r="D6">
-        <v>0.120099909916368</v>
+        <v>0.1261858979689367</v>
       </c>
       <c r="E6">
-        <v>0.30371421146953398</v>
+        <v>0.38181073277578648</v>
       </c>
       <c r="F6">
-        <v>8.7546180884109925E-2</v>
+        <v>0.1174411816009558</v>
       </c>
       <c r="G6">
-        <v>0.33924185145360408</v>
+        <v>0.37100408442851451</v>
       </c>
       <c r="H6">
-        <v>0.12606837108721619</v>
+        <v>0.1288478107526882</v>
       </c>
       <c r="I6">
-        <v>0.37769306152927129</v>
+        <v>0.4012607561017239</v>
       </c>
       <c r="J6">
-        <v>0.13024408422939071</v>
+        <v>0.1126826774193548</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -682,28 +744,28 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>0.3186647343687774</v>
+        <v>0.28282056272401429</v>
       </c>
       <c r="D7">
-        <v>0.1097955641577061</v>
+        <v>9.2343708960573465E-2</v>
       </c>
       <c r="E7">
-        <v>0.27000886260453999</v>
+        <v>0.2265720688968538</v>
       </c>
       <c r="F7">
-        <v>7.4062143130227007E-2</v>
+        <v>7.175436367980885E-2</v>
       </c>
       <c r="G7">
-        <v>0.3237500696933493</v>
+        <v>0.25743379729191562</v>
       </c>
       <c r="H7">
-        <v>0.1145830021505376</v>
+        <v>0.1046037954599761</v>
       </c>
       <c r="I7">
-        <v>0.38074566009557947</v>
+        <v>0.33027548088410991</v>
       </c>
       <c r="J7">
-        <v>0.1242511758832565</v>
+        <v>0.1029040325140809</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -714,28 +776,28 @@
         <v>15</v>
       </c>
       <c r="C8">
-        <v>0.34092719315013942</v>
+        <v>0.3186647343687774</v>
       </c>
       <c r="D8">
-        <v>0.1071180219832736</v>
+        <v>0.1097955641577061</v>
       </c>
       <c r="E8">
-        <v>0.30769531063321381</v>
+        <v>0.27000886260453999</v>
       </c>
       <c r="F8">
-        <v>7.763356463560335E-2</v>
+        <v>7.4062143130227007E-2</v>
       </c>
       <c r="G8">
-        <v>0.32889110155316609</v>
+        <v>0.3237500696933493</v>
       </c>
       <c r="H8">
-        <v>0.1072930659498208</v>
+        <v>0.1145830021505376</v>
       </c>
       <c r="I8">
-        <v>0.36244325098139613</v>
+        <v>0.38074566009557947</v>
       </c>
       <c r="J8">
-        <v>9.809929006656426E-2</v>
+        <v>0.1242511758832565</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -746,28 +808,28 @@
         <v>16</v>
       </c>
       <c r="C9">
-        <v>0.41324736758263642</v>
+        <v>0.30872469454400631</v>
       </c>
       <c r="D9">
-        <v>0.12749815675029871</v>
+        <v>8.7997688649940245E-2</v>
       </c>
       <c r="E9">
-        <v>0.35471768857029068</v>
+        <v>0.27046071166865798</v>
       </c>
       <c r="F9">
-        <v>0.1051770494623656</v>
+        <v>7.1315783990442069E-2</v>
       </c>
       <c r="G9">
-        <v>0.36381105894066113</v>
+        <v>0.2988493687773795</v>
       </c>
       <c r="H9">
-        <v>0.12547243990442061</v>
+        <v>0.100828680525687</v>
       </c>
       <c r="I9">
-        <v>0.41797175029868577</v>
+        <v>0.35154741167434722</v>
       </c>
       <c r="J9">
-        <v>0.1216317309267793</v>
+        <v>0.1059629395801331</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -778,28 +840,28 @@
         <v>17</v>
       </c>
       <c r="C10">
-        <v>0.36434364874551972</v>
+        <v>0.34092719315013942</v>
       </c>
       <c r="D10">
-        <v>0.1070808571087216</v>
+        <v>0.1071180219832736</v>
       </c>
       <c r="E10">
-        <v>0.29083403385105527</v>
+        <v>0.30769531063321381</v>
       </c>
       <c r="F10">
-        <v>7.0465027718040626E-2</v>
+        <v>7.763356463560335E-2</v>
       </c>
       <c r="G10">
-        <v>0.33143540342493027</v>
+        <v>0.32889110155316609</v>
       </c>
       <c r="H10">
-        <v>0.1056444339307049</v>
+        <v>0.1072930659498208</v>
       </c>
       <c r="I10">
-        <v>0.40202260582010579</v>
+        <v>0.36244325098139613</v>
       </c>
       <c r="J10">
-        <v>0.11319275345622121</v>
+        <v>9.809929006656426E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -810,28 +872,28 @@
         <v>18</v>
       </c>
       <c r="C11">
-        <v>0.36713684946236558</v>
+        <v>0.40658502349661491</v>
       </c>
       <c r="D11">
-        <v>0.1140524489844684</v>
+        <v>0.133054680525687</v>
       </c>
       <c r="E11">
-        <v>0.28934304380724812</v>
+        <v>0.35451344165671039</v>
       </c>
       <c r="F11">
-        <v>7.8925713261648753E-2</v>
+        <v>0.11408707311827949</v>
       </c>
       <c r="G11">
-        <v>0.33376081999203511</v>
+        <v>0.36084930426125061</v>
       </c>
       <c r="H11">
-        <v>0.1145908714456392</v>
+        <v>0.13215149486260461</v>
       </c>
       <c r="I11">
-        <v>0.39572908004778973</v>
+        <v>0.40695313150708318</v>
       </c>
       <c r="J11">
-        <v>0.1173318461341526</v>
+        <v>0.12382463159242189</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -842,28 +904,28 @@
         <v>19</v>
       </c>
       <c r="C12">
-        <v>0.39466196216646748</v>
+        <v>0.42521820788530468</v>
       </c>
       <c r="D12">
-        <v>0.1190324735961768</v>
+        <v>0.1244606697729988</v>
       </c>
       <c r="E12">
-        <v>0.32528437594583842</v>
+        <v>0.37771498287534838</v>
       </c>
       <c r="F12">
-        <v>9.0738510872162489E-2</v>
+        <v>0.1102721285543608</v>
       </c>
       <c r="G12">
-        <v>0.35242235364396662</v>
+        <v>0.38316936001592983</v>
       </c>
       <c r="H12">
-        <v>0.1197469111111111</v>
+        <v>0.12599141863799279</v>
       </c>
       <c r="I12">
-        <v>0.41910394393241168</v>
+        <v>0.40716517665130569</v>
       </c>
       <c r="J12">
-        <v>0.1194960299539171</v>
+        <v>0.1130760087045571</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -874,28 +936,28 @@
         <v>20</v>
       </c>
       <c r="C13">
-        <v>0.42521820788530468</v>
+        <v>0.31769913022700119</v>
       </c>
       <c r="D13">
-        <v>0.1244606697729988</v>
+        <v>0.1226002829151733</v>
       </c>
       <c r="E13">
-        <v>0.37771498287534838</v>
+        <v>0.26080937037037039</v>
       </c>
       <c r="F13">
-        <v>0.1102721285543608</v>
+        <v>7.8234182317801673E-2</v>
       </c>
       <c r="G13">
-        <v>0.38316936001592983</v>
+        <v>0.29062612704101948</v>
       </c>
       <c r="H13">
-        <v>0.12599141863799279</v>
+        <v>0.1203243992831541</v>
       </c>
       <c r="I13">
-        <v>0.40716517665130569</v>
+        <v>0.36399640809011768</v>
       </c>
       <c r="J13">
-        <v>0.1130760087045571</v>
+        <v>0.13593716615463389</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -906,28 +968,28 @@
         <v>21</v>
       </c>
       <c r="C14">
-        <v>0.40367119076065322</v>
+        <v>0.28966248387096782</v>
       </c>
       <c r="D14">
-        <v>0.1329511230585424</v>
+        <v>0.10492320908004781</v>
       </c>
       <c r="E14">
-        <v>0.35034039944245321</v>
+        <v>0.20662490123456789</v>
       </c>
       <c r="F14">
-        <v>0.1136679777777778</v>
+        <v>7.2926951254480288E-2</v>
       </c>
       <c r="G14">
-        <v>0.35596104659498212</v>
+        <v>0.25082501951413783</v>
       </c>
       <c r="H14">
-        <v>0.13273961720430111</v>
+        <v>0.1116878334528076</v>
       </c>
       <c r="I14">
-        <v>0.40630400110940429</v>
+        <v>0.34061422725721108</v>
       </c>
       <c r="J14">
-        <v>0.12482191730670759</v>
+        <v>0.1200607611367128</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -938,28 +1000,28 @@
         <v>22</v>
       </c>
       <c r="C15">
-        <v>0.41996924133811242</v>
+        <v>0.3125925786539227</v>
       </c>
       <c r="D15">
-        <v>0.1218930356033453</v>
+        <v>7.9993380406212664E-2</v>
       </c>
       <c r="E15">
-        <v>0.36449918518518509</v>
+        <v>0.25202684906411782</v>
       </c>
       <c r="F15">
-        <v>0.10455796200716851</v>
+        <v>6.7338230585424139E-2</v>
       </c>
       <c r="G15">
-        <v>0.37915904579848669</v>
+        <v>0.29334078255675028</v>
       </c>
       <c r="H15">
-        <v>0.1228442348864994</v>
+        <v>9.7413269772998801E-2</v>
       </c>
       <c r="I15">
-        <v>0.43280106246799788</v>
+        <v>0.35921848566308251</v>
       </c>
       <c r="J15">
-        <v>0.1174430401945725</v>
+        <v>9.4217673067076291E-2</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -970,28 +1032,28 @@
         <v>23</v>
       </c>
       <c r="C16">
-        <v>0.40658502349661491</v>
+        <v>0.40586848506571083</v>
       </c>
       <c r="D16">
-        <v>0.133054680525687</v>
+        <v>0.12603861242532849</v>
       </c>
       <c r="E16">
-        <v>0.35451344165671039</v>
+        <v>0.38385520469932288</v>
       </c>
       <c r="F16">
-        <v>0.11408707311827949</v>
+        <v>0.11816489581839899</v>
       </c>
       <c r="G16">
-        <v>0.36084930426125061</v>
+        <v>0.37423852608522501</v>
       </c>
       <c r="H16">
-        <v>0.13215149486260461</v>
+        <v>0.1297939178016726</v>
       </c>
       <c r="I16">
-        <v>0.40695313150708318</v>
+        <v>0.39426057176992663</v>
       </c>
       <c r="J16">
-        <v>0.12382463159242189</v>
+        <v>0.1117774126984127</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1002,28 +1064,28 @@
         <v>24</v>
       </c>
       <c r="C17">
-        <v>0.41117306730386288</v>
+        <v>0.39466196216646748</v>
       </c>
       <c r="D17">
-        <v>0.13151496917562719</v>
+        <v>0.1190324735961768</v>
       </c>
       <c r="E17">
-        <v>0.35771489884508167</v>
+        <v>0.32528437594583842</v>
       </c>
       <c r="F17">
-        <v>0.1127497758661888</v>
+        <v>9.0738510872162489E-2</v>
       </c>
       <c r="G17">
-        <v>0.36348772481083241</v>
+        <v>0.35242235364396662</v>
       </c>
       <c r="H17">
-        <v>0.12972741075268809</v>
+        <v>0.1197469111111111</v>
       </c>
       <c r="I17">
-        <v>0.41726091696535239</v>
+        <v>0.41910394393241168</v>
       </c>
       <c r="J17">
-        <v>0.12471186533538151</v>
+        <v>0.1194960299539171</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1034,28 +1096,28 @@
         <v>25</v>
       </c>
       <c r="C18">
-        <v>0.40252829948227792</v>
+        <v>0.31782991039426522</v>
       </c>
       <c r="D18">
-        <v>0.1276621199522103</v>
+        <v>9.1050570609318995E-2</v>
       </c>
       <c r="E18">
-        <v>0.33904976543209869</v>
+        <v>0.27428759936280372</v>
       </c>
       <c r="F18">
-        <v>0.1012916372759857</v>
+        <v>7.5601210513739539E-2</v>
       </c>
       <c r="G18">
-        <v>0.35010868657905209</v>
+        <v>0.29182108442851451</v>
       </c>
       <c r="H18">
-        <v>0.12502672329749101</v>
+        <v>0.107807576344086</v>
       </c>
       <c r="I18">
-        <v>0.41956464285714279</v>
+        <v>0.3619241816009558</v>
       </c>
       <c r="J18">
-        <v>0.124365051203277</v>
+        <v>0.10526507910906301</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1066,28 +1128,668 @@
         <v>26</v>
       </c>
       <c r="C19">
+        <v>0.41996924133811242</v>
+      </c>
+      <c r="D19">
+        <v>0.1218930356033453</v>
+      </c>
+      <c r="E19">
+        <v>0.36449918518518509</v>
+      </c>
+      <c r="F19">
+        <v>0.10455796200716851</v>
+      </c>
+      <c r="G19">
+        <v>0.37915904579848669</v>
+      </c>
+      <c r="H19">
+        <v>0.1228442348864994</v>
+      </c>
+      <c r="I19">
+        <v>0.43280106246799788</v>
+      </c>
+      <c r="J19">
+        <v>0.1174430401945725</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>0.34185133452807648</v>
+      </c>
+      <c r="D20">
+        <v>0.120099909916368</v>
+      </c>
+      <c r="E20">
+        <v>0.30371421146953398</v>
+      </c>
+      <c r="F20">
+        <v>8.7546180884109925E-2</v>
+      </c>
+      <c r="G20">
+        <v>0.33924185145360408</v>
+      </c>
+      <c r="H20">
+        <v>0.12606837108721619</v>
+      </c>
+      <c r="I20">
+        <v>0.37769306152927129</v>
+      </c>
+      <c r="J20">
+        <v>0.13024408422939071</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>0.35828716925527671</v>
+      </c>
+      <c r="D21">
+        <v>0.12592183058542411</v>
+      </c>
+      <c r="E21">
+        <v>0.30841619553962568</v>
+      </c>
+      <c r="F21">
+        <v>0.1049052191158901</v>
+      </c>
+      <c r="G21">
+        <v>0.33410105575467941</v>
+      </c>
+      <c r="H21">
+        <v>0.13192159689366789</v>
+      </c>
+      <c r="I21">
+        <v>0.38180538061102581</v>
+      </c>
+      <c r="J21">
+        <v>0.12809286277521759</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22">
         <v>0.34544052767821593</v>
       </c>
-      <c r="D19">
+      <c r="D22">
         <v>0.11954228339307051</v>
       </c>
-      <c r="E19">
+      <c r="E22">
         <v>0.24786641338112311</v>
       </c>
-      <c r="F19">
+      <c r="F22">
         <v>9.7465531660692939E-2</v>
       </c>
-      <c r="G19">
+      <c r="G22">
         <v>0.31596995459976113</v>
       </c>
-      <c r="H19">
+      <c r="H22">
         <v>0.1412421925925926</v>
       </c>
-      <c r="I19">
+      <c r="I22">
         <v>0.3865118322239291</v>
       </c>
-      <c r="J19">
+      <c r="J22">
         <v>0.14075010650281619</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23">
+        <v>0.27238327479091989</v>
+      </c>
+      <c r="D23">
+        <v>0.10800152401433689</v>
+      </c>
+      <c r="E23">
+        <v>0.24155350975706891</v>
+      </c>
+      <c r="F23">
+        <v>6.6075166547192352E-2</v>
+      </c>
+      <c r="G23">
+        <v>0.27196658821186781</v>
+      </c>
+      <c r="H23">
+        <v>0.10728013309438469</v>
+      </c>
+      <c r="I23">
+        <v>0.35598600273084152</v>
+      </c>
+      <c r="J23">
+        <v>0.12134669226830511</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24">
+        <v>0.32026751971326162</v>
+      </c>
+      <c r="D24">
+        <v>0.1044625844683393</v>
+      </c>
+      <c r="E24">
+        <v>0.26110407606531272</v>
+      </c>
+      <c r="F24">
+        <v>7.1898174910394255E-2</v>
+      </c>
+      <c r="G24">
+        <v>0.31357061529271207</v>
+      </c>
+      <c r="H24">
+        <v>0.1066021416965352</v>
+      </c>
+      <c r="I24">
+        <v>0.3784216705069125</v>
+      </c>
+      <c r="J24">
+        <v>0.1159565138248848</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>0.41324736758263642</v>
+      </c>
+      <c r="D25">
+        <v>0.12749815675029871</v>
+      </c>
+      <c r="E25">
+        <v>0.35471768857029068</v>
+      </c>
+      <c r="F25">
+        <v>0.1051770494623656</v>
+      </c>
+      <c r="G25">
+        <v>0.36381105894066113</v>
+      </c>
+      <c r="H25">
+        <v>0.12547243990442061</v>
+      </c>
+      <c r="I25">
+        <v>0.41797175029868577</v>
+      </c>
+      <c r="J25">
+        <v>0.1216317309267793</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26">
+        <v>0.41117306730386288</v>
+      </c>
+      <c r="D26">
+        <v>0.13151496917562719</v>
+      </c>
+      <c r="E26">
+        <v>0.35771489884508167</v>
+      </c>
+      <c r="F26">
+        <v>0.1127497758661888</v>
+      </c>
+      <c r="G26">
+        <v>0.36348772481083241</v>
+      </c>
+      <c r="H26">
+        <v>0.12972741075268809</v>
+      </c>
+      <c r="I26">
+        <v>0.41726091696535239</v>
+      </c>
+      <c r="J26">
+        <v>0.12471186533538151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>0.33303783671843878</v>
+      </c>
+      <c r="D27">
+        <v>0.10567916917562729</v>
+      </c>
+      <c r="E27">
+        <v>0.27764846395858228</v>
+      </c>
+      <c r="F27">
+        <v>6.7827279569892471E-2</v>
+      </c>
+      <c r="G27">
+        <v>0.30851121903624051</v>
+      </c>
+      <c r="H27">
+        <v>0.1091898138590203</v>
+      </c>
+      <c r="I27">
+        <v>0.37835753840245773</v>
+      </c>
+      <c r="J27">
+        <v>0.11339636354326681</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28">
+        <v>0.36434364874551972</v>
+      </c>
+      <c r="D28">
+        <v>0.1070808571087216</v>
+      </c>
+      <c r="E28">
+        <v>0.29083403385105527</v>
+      </c>
+      <c r="F28">
+        <v>7.0465027718040626E-2</v>
+      </c>
+      <c r="G28">
+        <v>0.33143540342493027</v>
+      </c>
+      <c r="H28">
+        <v>0.1056444339307049</v>
+      </c>
+      <c r="I28">
+        <v>0.40202260582010579</v>
+      </c>
+      <c r="J28">
+        <v>0.11319275345622121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29">
+        <v>0.40252829948227792</v>
+      </c>
+      <c r="D29">
+        <v>0.1276621199522103</v>
+      </c>
+      <c r="E29">
+        <v>0.33904976543209869</v>
+      </c>
+      <c r="F29">
+        <v>0.1012916372759857</v>
+      </c>
+      <c r="G29">
+        <v>0.35010868657905209</v>
+      </c>
+      <c r="H29">
+        <v>0.12502672329749101</v>
+      </c>
+      <c r="I29">
+        <v>0.41956464285714279</v>
+      </c>
+      <c r="J29">
+        <v>0.124365051203277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30">
+        <v>0.36713684946236558</v>
+      </c>
+      <c r="D30">
+        <v>0.1140524489844684</v>
+      </c>
+      <c r="E30">
+        <v>0.28934304380724812</v>
+      </c>
+      <c r="F30">
+        <v>7.8925713261648753E-2</v>
+      </c>
+      <c r="G30">
+        <v>0.33376081999203511</v>
+      </c>
+      <c r="H30">
+        <v>0.1145908714456392</v>
+      </c>
+      <c r="I30">
+        <v>0.39572908004778973</v>
+      </c>
+      <c r="J30">
+        <v>0.1173318461341526</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31">
+        <v>0.40367119076065322</v>
+      </c>
+      <c r="D31">
+        <v>0.1329511230585424</v>
+      </c>
+      <c r="E31">
+        <v>0.35034039944245321</v>
+      </c>
+      <c r="F31">
+        <v>0.1136679777777778</v>
+      </c>
+      <c r="G31">
+        <v>0.35596104659498212</v>
+      </c>
+      <c r="H31">
+        <v>0.13273961720430111</v>
+      </c>
+      <c r="I31">
+        <v>0.40630400110940429</v>
+      </c>
+      <c r="J31">
+        <v>0.12482191730670759</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32">
+        <v>0.28545257148546388</v>
+      </c>
+      <c r="D32">
+        <v>9.5809534528076459E-2</v>
+      </c>
+      <c r="E32">
+        <v>0.2150205523695739</v>
+      </c>
+      <c r="F32">
+        <v>7.4644783034647555E-2</v>
+      </c>
+      <c r="G32">
+        <v>0.25505418837116678</v>
+      </c>
+      <c r="H32">
+        <v>0.1065369913978495</v>
+      </c>
+      <c r="I32">
+        <v>0.34678538786482332</v>
+      </c>
+      <c r="J32">
+        <v>0.11359697977470561</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33">
+        <v>0.27118642134607718</v>
+      </c>
+      <c r="D33">
+        <v>9.4730189247311816E-2</v>
+      </c>
+      <c r="E33">
+        <v>0.19225094026284351</v>
+      </c>
+      <c r="F33">
+        <v>7.0605205017921155E-2</v>
+      </c>
+      <c r="G33">
+        <v>0.23421118598168059</v>
+      </c>
+      <c r="H33">
+        <v>0.10729649032258071</v>
+      </c>
+      <c r="I33">
+        <v>0.33075371693121691</v>
+      </c>
+      <c r="J33">
+        <v>0.1102367903225806</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34">
+        <v>0.28742656471525291</v>
+      </c>
+      <c r="D34">
+        <v>0.13885416821983271</v>
+      </c>
+      <c r="E34">
+        <v>0.26241724253285548</v>
+      </c>
+      <c r="F34">
+        <v>0.1140387906810036</v>
+      </c>
+      <c r="G34">
+        <v>0.2465983233771406</v>
+      </c>
+      <c r="H34">
+        <v>0.14380953620071679</v>
+      </c>
+      <c r="I34">
+        <v>0.26817943207031919</v>
+      </c>
+      <c r="J34">
+        <v>0.1139012657450077</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35">
+        <v>0.29878433373158098</v>
+      </c>
+      <c r="D35">
+        <v>0.13950407383512539</v>
+      </c>
+      <c r="E35">
+        <v>0.26141661210673039</v>
+      </c>
+      <c r="F35">
+        <v>0.11389629414575871</v>
+      </c>
+      <c r="G35">
+        <v>0.28619818797291918</v>
+      </c>
+      <c r="H35">
+        <v>0.15239372855436081</v>
+      </c>
+      <c r="I35">
+        <v>0.32245606332138588</v>
+      </c>
+      <c r="J35">
+        <v>0.144823194828469</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36">
+        <v>0.35530261847869382</v>
+      </c>
+      <c r="D36">
+        <v>0.1228047395459976</v>
+      </c>
+      <c r="E36">
+        <v>0.30836657228195941</v>
+      </c>
+      <c r="F36">
+        <v>0.1002377624850657</v>
+      </c>
+      <c r="G36">
+        <v>0.33429198128235771</v>
+      </c>
+      <c r="H36">
+        <v>0.12918153524492229</v>
+      </c>
+      <c r="I36">
+        <v>0.37724122802526022</v>
+      </c>
+      <c r="J36">
+        <v>0.123978404249872</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37">
+        <v>0.29209634846674631</v>
+      </c>
+      <c r="D37">
+        <v>0.10407190322580639</v>
+      </c>
+      <c r="E37">
+        <v>0.24039536280366389</v>
+      </c>
+      <c r="F37">
+        <v>6.262635101553167E-2</v>
+      </c>
+      <c r="G37">
+        <v>0.28377471166865792</v>
+      </c>
+      <c r="H37">
+        <v>0.1086817311827957</v>
+      </c>
+      <c r="I37">
+        <v>0.37913282130056319</v>
+      </c>
+      <c r="J37">
+        <v>0.117723065796211</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38">
+        <v>0.32756912345679012</v>
+      </c>
+      <c r="D38">
+        <v>9.7332529988052571E-2</v>
+      </c>
+      <c r="E38">
+        <v>0.26230201513341289</v>
+      </c>
+      <c r="F38">
+        <v>7.0104277419354835E-2</v>
+      </c>
+      <c r="G38">
+        <v>0.32110683074472318</v>
+      </c>
+      <c r="H38">
+        <v>0.10273956296296299</v>
+      </c>
+      <c r="I38">
+        <v>0.37596370327700979</v>
+      </c>
+      <c r="J38">
+        <v>0.111860513312852</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39">
+        <v>0.35536499522102738</v>
+      </c>
+      <c r="D39">
+        <v>8.8994540501792119E-2</v>
+      </c>
+      <c r="E39">
+        <v>0.296346847471127</v>
+      </c>
+      <c r="F39">
+        <v>7.0238719474313024E-2</v>
+      </c>
+      <c r="G39">
+        <v>0.33079598048586217</v>
+      </c>
+      <c r="H39">
+        <v>9.9134947670250884E-2</v>
+      </c>
+      <c r="I39">
+        <v>0.39432404761904771</v>
+      </c>
+      <c r="J39">
+        <v>9.4888290322580629E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>